<commit_message>
Add Uniprot Final Script
</commit_message>
<xml_diff>
--- a/BSR analysis/result.xlsx
+++ b/BSR analysis/result.xlsx
@@ -11,51 +11,6 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
-  <si>
-    <t>['ABK', 'EJZ', 'ESK', 'ETA', 'KEP']</t>
-  </si>
-  <si>
-    <t>ABK75244</t>
-  </si>
-  <si>
-    <t>Mycofactocin (Uncharacterized protein)</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-</t>
-  </si>
-  <si>
-    <t>EJZ10890</t>
-  </si>
-  <si>
-    <t>Uncharacterized protein</t>
-  </si>
-  <si>
-    <t>[' Mycofactocin.']</t>
-  </si>
-  <si>
-    <t>KEP43865</t>
-  </si>
-  <si>
-    <t>TetR family transcriptional regulator</t>
-  </si>
-  <si>
-    <t>ESK77308</t>
-  </si>
-  <si>
-    <t>Mycofactocin</t>
-  </si>
-  <si>
-    <t>ETA90315</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,103 +340,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A199:F204"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="199" spans="1:6">
-      <c r="A199" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6">
-      <c r="A200" t="s">
-        <v>1</v>
-      </c>
-      <c r="B200" t="s">
-        <v>2</v>
-      </c>
-      <c r="D200" t="s">
-        <v>3</v>
-      </c>
-      <c r="E200" t="s">
-        <v>3</v>
-      </c>
-      <c r="F200" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6">
-      <c r="A201" t="s">
-        <v>5</v>
-      </c>
-      <c r="B201" t="s">
-        <v>6</v>
-      </c>
-      <c r="D201" t="s">
-        <v>7</v>
-      </c>
-      <c r="E201" t="s">
-        <v>3</v>
-      </c>
-      <c r="F201" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6">
-      <c r="A202" t="s">
-        <v>8</v>
-      </c>
-      <c r="B202" t="s">
-        <v>9</v>
-      </c>
-      <c r="D202" t="s">
-        <v>7</v>
-      </c>
-      <c r="E202" t="s">
-        <v>3</v>
-      </c>
-      <c r="F202" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6">
-      <c r="A203" t="s">
-        <v>10</v>
-      </c>
-      <c r="B203" t="s">
-        <v>11</v>
-      </c>
-      <c r="D203" t="s">
-        <v>7</v>
-      </c>
-      <c r="E203" t="s">
-        <v>3</v>
-      </c>
-      <c r="F203" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6">
-      <c r="A204" t="s">
-        <v>12</v>
-      </c>
-      <c r="B204" t="s">
-        <v>9</v>
-      </c>
-      <c r="D204" t="s">
-        <v>7</v>
-      </c>
-      <c r="E204" t="s">
-        <v>3</v>
-      </c>
-      <c r="F204" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>